<commit_message>
add date select function.
</commit_message>
<xml_diff>
--- a/src/tmp/2021-03-23.xlsx
+++ b/src/tmp/2021-03-23.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,14 +472,140 @@
         <v>44278.60303240741</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>44278.65827546296</v>
+        <v>44278.60706018518</v>
       </c>
       <c r="D5" t="n">
-        <v>4773</v>
+        <v>348</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>extra</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2021-03-23</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>44278.60728009259</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>44278.63753472222</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2614</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2021-03-23</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>44278.64493055556</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>44278.68125</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3138</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2021-03-23</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>44278.69215277778</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>44278.7259837963</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2923</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2021-03-23</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>44278.85123842592</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>44278.8942824074</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3719</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2021-03-23</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>44278.90400462963</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>44278.92106481481</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1474</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2021-03-23</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>44278.92135416667</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>44278.93908564815</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1532</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>think</t>
         </is>
       </c>
     </row>
@@ -536,7 +662,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -576,7 +702,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -595,7 +721,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -620,6 +746,57 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2021-03-23</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>software</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>convenience</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2021-03-23</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>software</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>research</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2021-03-23</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>